<commit_message>
new page for parcelamentos and end-user interface enhancements
</commit_message>
<xml_diff>
--- a/regras_categorizacao.xlsx
+++ b/regras_categorizacao.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\99827109\Projetos\0.personal\analise-fatura-itau\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D7DAEF-9674-456B-8691-E314ADAD7912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE3D4A6-7E5C-4BED-B55A-707A7C46A805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
   <si>
     <t>PalavraChave</t>
   </si>
@@ -159,6 +159,186 @@
   </si>
   <si>
     <t>Almoço CSC</t>
+  </si>
+  <si>
+    <t>Raia Drogasil - NuPay</t>
+  </si>
+  <si>
+    <t>JAQUELINE DA SILVA</t>
+  </si>
+  <si>
+    <t>29192883000160 - Parcela 1/2</t>
+  </si>
+  <si>
+    <t>Luan de Oliveira Pegoraro</t>
+  </si>
+  <si>
+    <t>Szd Portal</t>
+  </si>
+  <si>
+    <t>Paes e Doces Center Chic Ltda Epp</t>
+  </si>
+  <si>
+    <t>Mercadolivre*4produto</t>
+  </si>
+  <si>
+    <t>sem Parar</t>
+  </si>
+  <si>
+    <t>Cacau Comercio Eletron - Parcela 1/2</t>
+  </si>
+  <si>
+    <t>Italoalunni</t>
+  </si>
+  <si>
+    <t>Estacionamento Fcr</t>
+  </si>
+  <si>
+    <t>Alo Bebe - Parcela 1/2</t>
+  </si>
+  <si>
+    <t>Ifd*Mercato Express Ho</t>
+  </si>
+  <si>
+    <t>Ifd*J C Gregorio Comer</t>
+  </si>
+  <si>
+    <t>SILVIA NASCIMENTO BARBOSA</t>
+  </si>
+  <si>
+    <t>Jacques Janine</t>
+  </si>
+  <si>
+    <t>Posto de Servicos Jd D</t>
+  </si>
+  <si>
+    <t>Drogasil1949</t>
+  </si>
+  <si>
+    <t>Mania de Churrasco Pri</t>
+  </si>
+  <si>
+    <t>Filipe dos Santos Cava</t>
+  </si>
+  <si>
+    <t>48752779aldaalves</t>
+  </si>
+  <si>
+    <t>Mp *Aliexpress - Parcela 1/4</t>
+  </si>
+  <si>
+    <t>Moda Mundial*Sheincom - Parcela 1/4</t>
+  </si>
+  <si>
+    <t>Ifd*Flying Butanta Com</t>
+  </si>
+  <si>
+    <t>Apple.Com/Bill</t>
+  </si>
+  <si>
+    <t>Amazon Retail Br Cpi - Parcela 1/3</t>
+  </si>
+  <si>
+    <t>Pagamento recebido</t>
+  </si>
+  <si>
+    <t>ZOOP BRASIL</t>
+  </si>
+  <si>
+    <t>Pg *Theminiforest - Parcela 6/6</t>
+  </si>
+  <si>
+    <t>Frizzon - Parcela 6/6</t>
+  </si>
+  <si>
+    <t>Fisia Nike Ecommer - Parcela 5/10</t>
+  </si>
+  <si>
+    <t>Sephoramorumbi - Parcela 5/5</t>
+  </si>
+  <si>
+    <t>Delboni Alto Pinheiros - Parcela 4/12</t>
+  </si>
+  <si>
+    <t>Rbbeauty Clinica de Es - Parcela 5/8</t>
+  </si>
+  <si>
+    <t>Bpg Crocs*Crocs Brasil - Parcela 2/2</t>
+  </si>
+  <si>
+    <t>Bpg Crocs*Crocs Brasil - Parcela 2/3</t>
+  </si>
+  <si>
+    <t>Agorasoumae - Parcela 6/6</t>
+  </si>
+  <si>
+    <t>App *Azurario - Parcela 4/12</t>
+  </si>
+  <si>
+    <t>Caps Analia Franco Com - Parcela 10/10</t>
+  </si>
+  <si>
+    <t>Pg *Medmanipulado Cedr - Parcela 2/2</t>
+  </si>
+  <si>
+    <t>Pg *Karoliny Lucas Pbc - Parcela 3/12</t>
+  </si>
+  <si>
+    <t>Alo Bebe - Parcela 2/2</t>
+  </si>
+  <si>
+    <t>SemParar</t>
+  </si>
+  <si>
+    <t>Ovo de Páscoa</t>
+  </si>
+  <si>
+    <t>Estacionamento</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Roupas Bebê</t>
+  </si>
+  <si>
+    <t>Pix</t>
+  </si>
+  <si>
+    <t>Silvia</t>
+  </si>
+  <si>
+    <t>Salão de Beleza</t>
+  </si>
+  <si>
+    <t>Gasolina</t>
+  </si>
+  <si>
+    <t>Almoço</t>
+  </si>
+  <si>
+    <t>Roupas Shein</t>
+  </si>
+  <si>
+    <t>Sushi</t>
+  </si>
+  <si>
+    <t>Roupas</t>
+  </si>
+  <si>
+    <t>Vacina Bronquio</t>
+  </si>
+  <si>
+    <t>Clínica Onodera</t>
+  </si>
+  <si>
+    <t>Presente Aniversário</t>
+  </si>
+  <si>
+    <t>Roupas Grávida</t>
+  </si>
+  <si>
+    <t>Compras Roupas Bebê</t>
   </si>
 </sst>
 </file>
@@ -176,15 +356,19 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -199,7 +383,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -207,24 +391,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,224 +684,606 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="45.28515625" style="5" customWidth="1"/>
+    <col min="2" max="3" width="27.5703125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>29192883000160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>